<commit_message>
investment number as dependent v
</commit_message>
<xml_diff>
--- a/2003-2023各省分行业全社会固定资产投资额.xlsx
+++ b/2003-2023各省分行业全社会固定资产投资额.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:dbsheet="http://web.wps.cn/et/2021/dbsheet">
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12255"/>
+    <workbookView windowWidth="29100" windowHeight="13540"/>
   </bookViews>
   <sheets>
     <sheet name="总数据" sheetId="1" r:id="rId1"/>
@@ -461,7 +461,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="855" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="855" uniqueCount="66">
   <si>
     <t>id</t>
   </si>
@@ -544,7 +544,7 @@
     <t>山西省</t>
   </si>
   <si>
-    <t>内蒙古自治区</t>
+    <t>内蒙古</t>
   </si>
   <si>
     <t>辽宁省</t>
@@ -589,7 +589,7 @@
     <t>广东省</t>
   </si>
   <si>
-    <t>广西壮族自治区</t>
+    <t>广西</t>
   </si>
   <si>
     <t>海南省</t>
@@ -607,7 +607,7 @@
     <t>云南省</t>
   </si>
   <si>
-    <t>西藏自治区</t>
+    <t>西藏</t>
   </si>
   <si>
     <t>陕西省</t>
@@ -619,10 +619,10 @@
     <t>青海省</t>
   </si>
   <si>
-    <t>宁夏回族自治区</t>
+    <t>宁夏</t>
   </si>
   <si>
-    <t>新疆维吾尔自治区</t>
+    <t>新疆</t>
   </si>
   <si>
     <t>10-18  分地区各行业固定资产投资比上年增长情况(2023年)</t>
@@ -632,6 +632,21 @@
   </si>
   <si>
     <t/>
+  </si>
+  <si>
+    <t>内蒙古自治区</t>
+  </si>
+  <si>
+    <t>广西壮族自治区</t>
+  </si>
+  <si>
+    <t>西藏自治区</t>
+  </si>
+  <si>
+    <t>宁夏回族自治区</t>
+  </si>
+  <si>
+    <t>新疆维吾尔自治区</t>
   </si>
   <si>
     <t>2018年后的数据根据官方公布的增长率计算得出！</t>
@@ -854,12 +869,12 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
       <sz val="9"/>
       <name val="宋体"/>
       <charset val="134"/>
     </font>
     <font>
+      <b/>
       <sz val="9"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -1708,35 +1723,35 @@
   <dimension ref="A1:W652"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C172" activePane="bottomRight" state="frozenSplit"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="K25" sqref="K25"/>
+      <selection pane="bottomRight" activeCell="C187" sqref="C187"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
   <cols>
-    <col min="1" max="2" width="8.89166666666667" style="4"/>
-    <col min="3" max="3" width="21.4833333333333" style="4" customWidth="1"/>
-    <col min="4" max="4" width="17.5583333333333" style="4"/>
-    <col min="5" max="5" width="16.4416666666667" style="4"/>
-    <col min="6" max="6" width="14.1083333333333" style="4"/>
-    <col min="7" max="8" width="16.4416666666667" style="4"/>
-    <col min="9" max="9" width="14.1083333333333" style="4"/>
-    <col min="10" max="10" width="12.8916666666667" style="4"/>
+    <col min="1" max="2" width="8.89285714285714" style="4"/>
+    <col min="3" max="3" width="21.4821428571429" style="4" customWidth="1"/>
+    <col min="4" max="4" width="17.5625" style="4"/>
+    <col min="5" max="5" width="16.4375" style="4"/>
+    <col min="6" max="6" width="14.1071428571429" style="4"/>
+    <col min="7" max="8" width="16.4375" style="4"/>
+    <col min="9" max="9" width="14.1071428571429" style="4"/>
+    <col min="10" max="10" width="12.8928571428571" style="4"/>
     <col min="11" max="11" width="13" style="4"/>
-    <col min="12" max="12" width="12.8916666666667" style="4"/>
-    <col min="13" max="13" width="12.8916666666667" style="6"/>
+    <col min="12" max="12" width="12.8928571428571" style="4"/>
+    <col min="13" max="13" width="12.8928571428571" style="6"/>
     <col min="14" max="14" width="13.75" style="4"/>
-    <col min="15" max="15" width="14.1083333333333" style="4"/>
+    <col min="15" max="15" width="14.1071428571429" style="4"/>
     <col min="16" max="16" width="13" style="4"/>
-    <col min="17" max="17" width="12.8916666666667" style="4"/>
+    <col min="17" max="17" width="12.8928571428571" style="4"/>
     <col min="18" max="18" width="13" style="4"/>
-    <col min="19" max="20" width="12.8916666666667" style="4"/>
+    <col min="19" max="20" width="12.8928571428571" style="4"/>
     <col min="21" max="21" width="13" style="4"/>
-    <col min="22" max="23" width="12.8916666666667" style="4"/>
-    <col min="24" max="16384" width="8.89166666666667" style="4"/>
+    <col min="22" max="23" width="12.8928571428571" style="4"/>
+    <col min="24" max="16384" width="8.89285714285714" style="4"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="1" ht="97.2" customHeight="1" spans="1:23">
@@ -14394,7 +14409,7 @@
         <v>268.441</v>
       </c>
       <c r="F179" s="4">
-        <v>205.2774</v>
+        <v>268.441</v>
       </c>
       <c r="G179" s="4">
         <v>2018.6186</v>
@@ -23292,7 +23307,6 @@
       <c r="M304" s="6">
         <v>6.3837</v>
       </c>
-      <c r="N304" s="4"/>
       <c r="O304" s="4">
         <v>1859.3143</v>
       </c>
@@ -25618,7 +25632,6 @@
       <c r="H337" s="4">
         <v>170.6021</v>
       </c>
-      <c r="I337" s="4"/>
       <c r="J337" s="4">
         <v>18.8324</v>
       </c>
@@ -27817,7 +27830,6 @@
       <c r="H368" s="4">
         <v>232.2407</v>
       </c>
-      <c r="I368" s="4"/>
       <c r="J368" s="4">
         <v>9.1694</v>
       </c>
@@ -31877,7 +31889,6 @@
       <c r="M425" s="6">
         <v>88.4129</v>
       </c>
-      <c r="N425" s="4"/>
       <c r="O425" s="4">
         <v>2117.991</v>
       </c>
@@ -34872,7 +34883,6 @@
       <c r="R467" s="4">
         <v>740.0194</v>
       </c>
-      <c r="S467" s="4"/>
       <c r="T467" s="4">
         <v>125.7329</v>
       </c>
@@ -41423,7 +41433,6 @@
       <c r="R560" s="4">
         <v>486.742730427054</v>
       </c>
-      <c r="S560" s="4"/>
       <c r="T560" s="4">
         <v>173.099491866449</v>
       </c>
@@ -41672,7 +41681,6 @@
       <c r="H564" s="4">
         <v>1637.75492612433</v>
       </c>
-      <c r="I564" s="4"/>
       <c r="J564" s="4">
         <v>63.7552905678625</v>
       </c>
@@ -41741,7 +41749,6 @@
       <c r="H565" s="4">
         <v>661.460486124403</v>
       </c>
-      <c r="I565" s="4"/>
       <c r="J565" s="4">
         <v>59.1605352695649</v>
       </c>
@@ -41810,7 +41817,6 @@
       <c r="H566" s="4">
         <v>567.72349954372</v>
       </c>
-      <c r="I566" s="4"/>
       <c r="J566" s="4">
         <v>116.288707732956</v>
       </c>
@@ -41876,7 +41882,6 @@
       <c r="H567" s="4">
         <v>855.389419193323</v>
       </c>
-      <c r="I567" s="4"/>
       <c r="J567" s="4">
         <v>260.952267052125</v>
       </c>
@@ -41936,14 +41941,12 @@
       <c r="E568" s="4">
         <v>24.003054</v>
       </c>
-      <c r="F568" s="4"/>
       <c r="G568" s="4">
         <v>1433.5552876425</v>
       </c>
       <c r="H568" s="4">
         <v>262.772635443801</v>
       </c>
-      <c r="I568" s="4"/>
       <c r="J568" s="4">
         <v>17.4212910925501</v>
       </c>
@@ -42784,7 +42787,6 @@
       <c r="E580" s="4">
         <v>94.3374912130352</v>
       </c>
-      <c r="F580" s="4"/>
       <c r="G580" s="4">
         <v>276.692719539845</v>
       </c>
@@ -43286,7 +43288,6 @@
       <c r="H587" s="4">
         <v>643.811869088435</v>
       </c>
-      <c r="I587" s="4"/>
       <c r="J587" s="4">
         <v>102.381804776378</v>
       </c>
@@ -43426,7 +43427,6 @@
       <c r="H589" s="4">
         <v>333.00779836197</v>
       </c>
-      <c r="I589" s="4"/>
       <c r="J589" s="4">
         <v>26.2225054431454</v>
       </c>
@@ -43439,7 +43439,6 @@
       <c r="M589" s="4">
         <v>31.8023082983522</v>
       </c>
-      <c r="N589" s="4"/>
       <c r="O589" s="4">
         <v>535.784656213346</v>
       </c>
@@ -43594,7 +43593,6 @@
       <c r="R591" s="4">
         <v>440.502171036484</v>
       </c>
-      <c r="S591" s="4"/>
       <c r="T591" s="4">
         <v>195.602425809087</v>
       </c>
@@ -43633,7 +43631,6 @@
       <c r="H592" s="4">
         <v>429.671003145849</v>
       </c>
-      <c r="I592" s="4"/>
       <c r="J592" s="4">
         <v>142.503465318868</v>
       </c>
@@ -43844,7 +43841,6 @@
       <c r="H595" s="4">
         <v>2571.2752340152</v>
       </c>
-      <c r="I595" s="4"/>
       <c r="J595" s="4">
         <v>81.9893036702712</v>
       </c>
@@ -43913,7 +43909,6 @@
       <c r="H596" s="4">
         <v>773.247308279427</v>
       </c>
-      <c r="I596" s="4"/>
       <c r="J596" s="4">
         <v>57.5040402820171</v>
       </c>
@@ -43982,7 +43977,6 @@
       <c r="H597" s="4">
         <v>770.968512380371</v>
       </c>
-      <c r="I597" s="4"/>
       <c r="J597" s="4">
         <v>241.066491130419</v>
       </c>
@@ -44048,7 +44042,6 @@
       <c r="H598" s="4">
         <v>859.66636628929</v>
       </c>
-      <c r="I598" s="4"/>
       <c r="J598" s="4">
         <v>356.721749060255</v>
       </c>
@@ -44108,14 +44101,12 @@
       <c r="E599" s="4">
         <v>8.737111656</v>
       </c>
-      <c r="F599" s="4"/>
       <c r="G599" s="4">
         <v>1463.65994868299</v>
       </c>
       <c r="H599" s="4">
         <v>243.853005691847</v>
       </c>
-      <c r="I599" s="4"/>
       <c r="J599" s="4">
         <v>10.3830894911599</v>
       </c>
@@ -44956,7 +44947,6 @@
       <c r="E611" s="4">
         <v>106.507027579517</v>
       </c>
-      <c r="F611" s="4"/>
       <c r="G611" s="4">
         <v>335.074883362752</v>
       </c>
@@ -45458,7 +45448,6 @@
       <c r="H618" s="4">
         <v>1141.4784438938</v>
       </c>
-      <c r="I618" s="4"/>
       <c r="J618" s="4">
         <v>107.193749600867</v>
       </c>
@@ -45598,7 +45587,6 @@
       <c r="H620" s="4">
         <v>389.952131881866</v>
       </c>
-      <c r="I620" s="4"/>
       <c r="J620" s="4">
         <v>33.4336944400104</v>
       </c>
@@ -45736,7 +45724,6 @@
       <c r="H622" s="4">
         <v>239.599282378094</v>
       </c>
-      <c r="I622" s="4"/>
       <c r="J622" s="4">
         <v>11.713092412254</v>
       </c>
@@ -45764,7 +45751,6 @@
       <c r="R622" s="4">
         <v>482.790379455987</v>
       </c>
-      <c r="S622" s="4"/>
       <c r="T622" s="4">
         <v>172.521339563615</v>
       </c>
@@ -45803,7 +45789,6 @@
       <c r="H623" s="4">
         <v>491.113956595705</v>
       </c>
-      <c r="I623" s="4"/>
       <c r="J623" s="4">
         <v>344.003365279747</v>
       </c>
@@ -46014,7 +45999,6 @@
       <c r="H626" s="4">
         <v>3280.9471986034</v>
       </c>
-      <c r="I626" s="4"/>
       <c r="J626" s="4">
         <v>88.7124265712334</v>
       </c>
@@ -46083,7 +46067,6 @@
       <c r="H627" s="4">
         <v>969.652124582401</v>
       </c>
-      <c r="I627" s="4"/>
       <c r="J627" s="4">
         <v>53.4212534219939</v>
       </c>
@@ -46152,7 +46135,6 @@
       <c r="H628" s="4">
         <v>831.87502485842</v>
       </c>
-      <c r="I628" s="4"/>
       <c r="J628" s="4">
         <v>107.997788026428</v>
       </c>
@@ -46216,7 +46198,6 @@
       <c r="H629" s="4">
         <v>786.5947251547</v>
       </c>
-      <c r="I629" s="4"/>
       <c r="J629" s="4">
         <v>319.265965408928</v>
       </c>
@@ -46276,14 +46257,12 @@
       <c r="E630" s="4">
         <v>9.706931049816</v>
       </c>
-      <c r="F630" s="4"/>
       <c r="G630" s="4">
         <v>1561.31534045912</v>
       </c>
       <c r="H630" s="4">
         <v>222.881647202348</v>
       </c>
-      <c r="I630" s="4"/>
       <c r="J630" s="4">
         <v>20.2470245077618</v>
       </c>
@@ -46636,7 +46615,6 @@
       <c r="H635" s="4">
         <v>823.86095618639</v>
       </c>
-      <c r="I635" s="4"/>
       <c r="J635" s="4">
         <v>476.652045411317</v>
       </c>
@@ -46776,7 +46754,6 @@
       <c r="H637" s="4">
         <v>2992.20798598424</v>
       </c>
-      <c r="I637" s="4"/>
       <c r="J637" s="4">
         <v>833.125743554889</v>
       </c>
@@ -47120,14 +47097,12 @@
       <c r="E642" s="4">
         <v>78.8152004088426</v>
       </c>
-      <c r="F642" s="4"/>
       <c r="G642" s="4">
         <v>282.685925348986</v>
       </c>
       <c r="H642" s="4">
         <v>350.049018870975</v>
       </c>
-      <c r="I642" s="4"/>
       <c r="J642" s="4">
         <v>11.4841651591919</v>
       </c>
@@ -47211,7 +47186,6 @@
       <c r="M643" s="4">
         <v>281.710510990257</v>
       </c>
-      <c r="N643" s="4"/>
       <c r="O643" s="4">
         <v>3429.69304865719</v>
       </c>
@@ -47491,7 +47465,6 @@
         <v>32.2863539918902</v>
       </c>
       <c r="M647" s="4"/>
-      <c r="N647" s="4"/>
       <c r="O647" s="4">
         <v>233.791407723361</v>
       </c>
@@ -47616,7 +47589,6 @@
       <c r="H649" s="4">
         <v>1498.76119683256</v>
       </c>
-      <c r="I649" s="4"/>
       <c r="J649" s="4">
         <v>197.986855512801</v>
       </c>
@@ -47700,7 +47672,6 @@
       <c r="M650" s="4">
         <v>35.0792419965218</v>
       </c>
-      <c r="N650" s="4"/>
       <c r="O650" s="4">
         <v>356.969532402499</v>
       </c>
@@ -47754,7 +47725,6 @@
       <c r="H651" s="4">
         <v>526.825330172401</v>
       </c>
-      <c r="I651" s="4"/>
       <c r="J651" s="4">
         <v>32.02947927353</v>
       </c>
@@ -47767,7 +47737,6 @@
       <c r="M651" s="4">
         <v>54.5391778024092</v>
       </c>
-      <c r="N651" s="4"/>
       <c r="O651" s="4">
         <v>499.155202406665</v>
       </c>
@@ -47892,7 +47861,7 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
   <cols>
     <col min="3" max="3" width="16" customWidth="1"/>
     <col min="4" max="4" width="13.75"/>
@@ -48271,7 +48240,7 @@
         <v>2023</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>27</v>
+        <v>57</v>
       </c>
       <c r="D9">
         <v>19.833</v>
@@ -49336,7 +49305,7 @@
         <v>2023</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="D24">
         <v>-15.451</v>
@@ -49762,7 +49731,7 @@
         <v>2023</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="D30">
         <v>35.074</v>
@@ -50046,7 +50015,7 @@
         <v>2023</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="D34">
         <v>5.543</v>
@@ -50117,7 +50086,7 @@
         <v>2023</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="D35">
         <v>12.432</v>
@@ -50180,7 +50149,7 @@
         <v>-10.8</v>
       </c>
     </row>
-    <row r="39" ht="78.75" spans="1:23">
+    <row r="39" ht="124" spans="1:23">
       <c r="A39" s="2" t="s">
         <v>0</v>
       </c>
@@ -50539,7 +50508,7 @@
         <v>2022</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>27</v>
+        <v>57</v>
       </c>
       <c r="D44" s="4">
         <v>13635.1944843686</v>
@@ -51590,7 +51559,7 @@
         <v>2022</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="D59" s="4">
         <v>27926.871174291</v>
@@ -52014,7 +51983,7 @@
         <v>2022</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="D65" s="4">
         <v>1573.629404365</v>
@@ -52294,7 +52263,7 @@
         <v>2022</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="D69" s="4">
         <v>3204.69945791806</v>
@@ -52361,7 +52330,7 @@
         <v>2022</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="D70" s="4">
         <v>13327.1199109402</v>
@@ -52424,7 +52393,7 @@
         <v>156.648764628812</v>
       </c>
     </row>
-    <row r="74" ht="78.75" spans="1:23">
+    <row r="74" ht="124" spans="1:23">
       <c r="A74" s="2" t="s">
         <v>0</v>
       </c>
@@ -52858,7 +52827,7 @@
         <v>2023</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>27</v>
+        <v>57</v>
       </c>
       <c r="D79" s="4">
         <f t="shared" si="1"/>
@@ -54193,7 +54162,7 @@
         <v>2023</v>
       </c>
       <c r="C94" s="4" t="s">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="D94" s="4">
         <f t="shared" si="1"/>
@@ -54730,7 +54699,7 @@
         <v>2023</v>
       </c>
       <c r="C100" s="4" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="D100" s="4">
         <f t="shared" si="1"/>
@@ -55082,7 +55051,7 @@
         <v>2023</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="D104" s="4">
         <f t="shared" si="1"/>
@@ -55167,7 +55136,7 @@
         <v>2023</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="D105" s="4">
         <f t="shared" si="1"/>
@@ -55266,35 +55235,35 @@
       <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
   <cols>
     <col min="1" max="1" width="69.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:1">
+    <row r="2" ht="17" spans="1:1">
       <c r="A2" s="1" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="1"/>
     </row>
-    <row r="4" ht="28.5" spans="1:1">
+    <row r="4" ht="34" spans="1:1">
       <c r="A4" s="1" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="1"/>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" ht="17" spans="1:1">
       <c r="A6" s="1" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>